<commit_message>
Ajout d'une nouvelle page pour l'analyse de données, phase 1
</commit_message>
<xml_diff>
--- a/frontend/dashboard/src/assets/Classeur.xlsx
+++ b/frontend/dashboard/src/assets/Classeur.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar Boutoile777\Connexion\new\importation_exel_in_postgresql_\frontend\dashboard\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43145F95-B103-4C64-BEFD-C095CE766760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6582CD-9CBA-4206-9192-072785C27ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70ACAB68-A8F1-4978-9AD0-52B60AE6191C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{70ACAB68-A8F1-4978-9AD0-52B60AE6191C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,76 +26,180 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>date_comite_validation</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>pda</t>
   </si>
   <si>
-    <t>psf</t>
-  </si>
-  <si>
-    <t>departement</t>
-  </si>
-  <si>
     <t>commune</t>
   </si>
   <si>
-    <t>intitule_projet</t>
-  </si>
-  <si>
-    <t>denomination_entite</t>
-  </si>
-  <si>
-    <t>nom_promoteur</t>
-  </si>
-  <si>
-    <t>sexe_promoteur</t>
-  </si>
-  <si>
-    <t>statut_juridique</t>
-  </si>
-  <si>
-    <t>adresse_contact</t>
-  </si>
-  <si>
-    <t>filiere</t>
-  </si>
-  <si>
-    <t>maillon_type_credit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cout_total_projet </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> credit_solicite </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> credit_accorde </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> refinancement_accorde </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> credit_accorde_statut </t>
-  </si>
-  <si>
-    <t>total_financement</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> statut_dossier </t>
+    <t>Date comité de validation</t>
+  </si>
+  <si>
+    <t>N° dossier</t>
+  </si>
+  <si>
+    <t>Nom PSF</t>
+  </si>
+  <si>
+    <t>Département</t>
+  </si>
+  <si>
+    <t>Intitulé du projet</t>
+  </si>
+  <si>
+    <t>Nom de l'entité</t>
+  </si>
+  <si>
+    <t>Nom du promoteur</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t>Statut juridique</t>
+  </si>
+  <si>
+    <t>Adresse/contact</t>
+  </si>
+  <si>
+    <t>Rang/Cycles</t>
+  </si>
+  <si>
+    <t>Filière</t>
+  </si>
+  <si>
+    <t>Maillon/type crédit</t>
+  </si>
+  <si>
+    <t>Coût total</t>
+  </si>
+  <si>
+    <t>Crédit sollicité</t>
+  </si>
+  <si>
+    <t>Crédit accordé</t>
+  </si>
+  <si>
+    <t>Refinancement accordé</t>
+  </si>
+  <si>
+    <t>Statut crédit accordé</t>
+  </si>
+  <si>
+    <t>Total financement</t>
+  </si>
+  <si>
+    <t>Statut dossier</t>
+  </si>
+  <si>
+    <t>Garantie FNDA accordée</t>
+  </si>
+  <si>
+    <t>Bonification FNDA accordée</t>
+  </si>
+  <si>
+    <t>MOTIF si crédit non accordé</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Référence si notifié</t>
+  </si>
+  <si>
+    <t>Date de notification</t>
+  </si>
+  <si>
+    <t>Montant décaissé</t>
+  </si>
+  <si>
+    <t>Date de création de l'entité</t>
+  </si>
+  <si>
+    <t>NPI</t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Commune</t>
+  </si>
+  <si>
+    <t>PDA</t>
+  </si>
+  <si>
+    <t>Nom SFD</t>
+  </si>
+  <si>
+    <t>Date de décaissement</t>
+  </si>
+  <si>
+    <t>Noms du groupe/groupement/MPME/individu/…</t>
+  </si>
+  <si>
+    <t>Noms des bénéficiaires</t>
+  </si>
+  <si>
+    <t>Nombre de bénéficiaire homme</t>
+  </si>
+  <si>
+    <t>Nombre de bénéficiaire femme</t>
+  </si>
+  <si>
+    <t>Total bénéficiaire</t>
+  </si>
+  <si>
+    <t>Nom du responsable</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Objet du crédits</t>
+  </si>
+  <si>
+    <t>Type crédits</t>
+  </si>
+  <si>
+    <t>Montant sollicité</t>
+  </si>
+  <si>
+    <t>Chiffre d'Affaire annuel</t>
+  </si>
+  <si>
+    <t>Montant accordé</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>Différé (mois)</t>
+  </si>
+  <si>
+    <t>Périodicité de remboursement</t>
+  </si>
+  <si>
+    <t>Date première échéance</t>
+  </si>
+  <si>
+    <t>Date dernière échéance</t>
+  </si>
+  <si>
+    <t>Observations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot; &quot;#,##0&quot;   &quot;;&quot;-&quot;#,##0&quot;   &quot;;&quot; -&quot;00&quot;   &quot;;&quot; &quot;@&quot; &quot;"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +215,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +246,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FFC6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFC6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,16 +292,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Milliers [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,52 +631,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60671AB1-D2BA-4806-BB00-28DF9FBC0775}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
     <col min="8" max="8" width="22.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="15.88671875" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
     <col min="14" max="14" width="20.77734375" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" customWidth="1"/>
     <col min="16" max="16" width="14.5546875" customWidth="1"/>
     <col min="17" max="17" width="14.88671875" customWidth="1"/>
     <col min="18" max="18" width="23.88671875" customWidth="1"/>
-    <col min="19" max="19" width="21.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="21" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" customWidth="1"/>
+    <col min="23" max="23" width="29.88671875" customWidth="1"/>
+    <col min="24" max="24" width="31" customWidth="1"/>
+    <col min="25" max="25" width="32.21875" customWidth="1"/>
+    <col min="26" max="26" width="18.44140625" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" customWidth="1"/>
+    <col min="28" max="28" width="24.77734375" customWidth="1"/>
+    <col min="29" max="29" width="18.88671875" customWidth="1"/>
+    <col min="30" max="30" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -562,10 +732,167 @@
       </c>
       <c r="U1" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EC01B-626D-4784-BED2-41E520E1202F}">
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="48.88671875" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" customWidth="1"/>
+    <col min="10" max="10" width="32.21875" customWidth="1"/>
+    <col min="11" max="11" width="31.77734375" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" customWidth="1"/>
+    <col min="14" max="14" width="26.21875" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="24" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" customWidth="1"/>
+    <col min="19" max="19" width="19.21875" customWidth="1"/>
+    <col min="20" max="20" width="27.33203125" customWidth="1"/>
+    <col min="21" max="21" width="18.88671875" customWidth="1"/>
+    <col min="23" max="23" width="21.44140625" customWidth="1"/>
+    <col min="24" max="24" width="31.21875" customWidth="1"/>
+    <col min="25" max="25" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>